<commit_message>
VM load state from WS and update View
</commit_message>
<xml_diff>
--- a/Source.xlsx
+++ b/Source.xlsx
@@ -8,13 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\excel-related-table-tool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFA3402E-C0D3-4B46-B062-A24C4A0A6EE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{578483F9-2817-476F-AE25-BB8AB5F186AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="173">
   <si>
     <t>Rank</t>
   </si>
@@ -552,18 +551,6 @@
   </si>
   <si>
     <t>Tan Son Nhat International Airport</t>
-  </si>
-  <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>b</t>
-  </si>
-  <si>
-    <t>Column1</t>
-  </si>
-  <si>
-    <t>Column2</t>
   </si>
 </sst>
 </file>
@@ -636,17 +623,6 @@
     <tableColumn id="3" xr3:uid="{9E69402D-507A-4F6F-A598-A9C4B709A055}" name="Location"/>
     <tableColumn id="5" xr3:uid="{CF946CBC-DCBB-44D5-8FAD-CBED678A8EB7}" name="Code"/>
     <tableColumn id="6" xr3:uid="{E269B006-49D3-427B-B4BC-F583EE1ED5BF}" name="Total passengers" dataDxfId="0"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{427485BB-2F85-4663-BA94-237F492DFD28}" name="Table2" displayName="Table2" ref="A1:B3" totalsRowShown="0">
-  <autoFilter ref="A1:B3" xr:uid="{427485BB-2F85-4663-BA94-237F492DFD28}"/>
-  <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{76280E03-A631-437B-BB46-E9ACBC9FCA34}" name="Column1"/>
-    <tableColumn id="2" xr3:uid="{1224CC23-A8C6-4858-96D9-3CA38B20FCDF}" name="Column2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -918,8 +894,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:F53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1964,47 +1940,4 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CC6AD32-3B1E-469D-A7EB-D7CAC05C1FF4}">
-  <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:B3"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="2" width="11" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>175</v>
-      </c>
-      <c r="B1" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>173</v>
-      </c>
-      <c r="B2" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>174</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
 </file>
</xml_diff>